<commit_message>
Chrome and Firefoxe browsers in parameters
</commit_message>
<xml_diff>
--- a/src/test/java/common/test_data/users/Users.xlsx
+++ b/src/test/java/common/test_data/users/Users.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -61,6 +61,33 @@
   </si>
   <si>
     <t>TestPassw0rd@123!$RrRKuBeIod</t>
+  </si>
+  <si>
+    <t>TestUser_1ASltkyXYuI</t>
+  </si>
+  <si>
+    <t>automation_test+1611390700+afMLZuyHBy@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPassw0rd@123!$wAFQkDdmos</t>
+  </si>
+  <si>
+    <t>TestUser_1mevqxjIwaa</t>
+  </si>
+  <si>
+    <t>automation_test+1611426616+mzWnKOpXgz@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPassw0rd@123!$bSYYzpxNUl</t>
+  </si>
+  <si>
+    <t>TestUser_1EpFdZwhfiQ</t>
+  </si>
+  <si>
+    <t>automation_test+1611426867+bLXuuqccZE@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPassw0rd@123!$fIRELWtCja</t>
   </si>
 </sst>
 </file>
@@ -426,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F8A7C7-837A-425F-9758-BEEBC1A7DFF8}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
@@ -472,6 +499,39 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
DataProvider added + NullPointerException handler
</commit_message>
<xml_diff>
--- a/src/test/java/common/test_data/users/Users.xlsx
+++ b/src/test/java/common/test_data/users/Users.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>TestPassw0rd@123!$fIRELWtCja</t>
+  </si>
+  <si>
+    <t>TestUser_1DKUKxoJrIT</t>
+  </si>
+  <si>
+    <t>automation_test+1611435001+RuarLPPYUp@gmail.com</t>
+  </si>
+  <si>
+    <t>TestPassw0rd@123!$lOOtqQERdv</t>
   </si>
 </sst>
 </file>
@@ -453,7 +462,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F8A7C7-837A-425F-9758-BEEBC1A7DFF8}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
@@ -532,6 +541,17 @@
         <v>17</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>